<commit_message>
fixed possible bug in test level for projectiles
</commit_message>
<xml_diff>
--- a/Assets/Resources/TestLevel1_Proj.xlsx
+++ b/Assets/Resources/TestLevel1_Proj.xlsx
@@ -13,10 +13,6 @@
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -355,8 +351,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D88" sqref="D88"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38:C89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -887,7 +883,7 @@
         <v>25.25</v>
       </c>
       <c r="C38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D38">
         <v>3</v>
@@ -901,7 +897,7 @@
         <v>25.5</v>
       </c>
       <c r="C39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D39">
         <v>2</v>
@@ -915,7 +911,7 @@
         <v>25.75</v>
       </c>
       <c r="C40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D40">
         <v>4</v>
@@ -929,7 +925,7 @@
         <v>28</v>
       </c>
       <c r="C41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D41">
         <v>2</v>
@@ -943,7 +939,7 @@
         <v>28.25</v>
       </c>
       <c r="C42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D42">
         <v>2</v>
@@ -957,7 +953,7 @@
         <v>28.5</v>
       </c>
       <c r="C43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D43">
         <v>2</v>
@@ -971,7 +967,7 @@
         <v>28.75</v>
       </c>
       <c r="C44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D44">
         <v>2</v>
@@ -985,7 +981,7 @@
         <v>29</v>
       </c>
       <c r="C45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D45">
         <v>2</v>
@@ -999,7 +995,7 @@
         <v>29.25</v>
       </c>
       <c r="C46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D46">
         <v>2</v>
@@ -1013,7 +1009,7 @@
         <v>29.5</v>
       </c>
       <c r="C47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D47">
         <v>2</v>
@@ -1027,7 +1023,7 @@
         <v>29.75</v>
       </c>
       <c r="C48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D48">
         <v>2</v>
@@ -1041,7 +1037,7 @@
         <v>30</v>
       </c>
       <c r="C49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D49">
         <v>2</v>
@@ -1055,7 +1051,7 @@
         <v>30.25</v>
       </c>
       <c r="C50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D50">
         <v>2</v>
@@ -1069,7 +1065,7 @@
         <v>30.5</v>
       </c>
       <c r="C51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D51">
         <v>2</v>
@@ -1083,7 +1079,7 @@
         <v>30.75</v>
       </c>
       <c r="C52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D52">
         <v>2</v>
@@ -1097,7 +1093,7 @@
         <v>31</v>
       </c>
       <c r="C53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D53">
         <v>2</v>
@@ -1111,7 +1107,7 @@
         <v>31.25</v>
       </c>
       <c r="C54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D54">
         <v>2</v>
@@ -1125,7 +1121,7 @@
         <v>31.5</v>
       </c>
       <c r="C55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D55">
         <v>2</v>
@@ -1139,7 +1135,7 @@
         <v>31.75</v>
       </c>
       <c r="C56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D56">
         <v>2</v>
@@ -1153,7 +1149,7 @@
         <v>32</v>
       </c>
       <c r="C57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D57">
         <v>2</v>
@@ -1167,7 +1163,7 @@
         <v>32.25</v>
       </c>
       <c r="C58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D58">
         <v>2</v>
@@ -1181,7 +1177,7 @@
         <v>32.5</v>
       </c>
       <c r="C59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D59">
         <v>2</v>
@@ -1195,7 +1191,7 @@
         <v>32.75</v>
       </c>
       <c r="C60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D60">
         <v>2</v>
@@ -1209,7 +1205,7 @@
         <v>33</v>
       </c>
       <c r="C61">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D61">
         <v>2</v>
@@ -1223,7 +1219,7 @@
         <v>33.25</v>
       </c>
       <c r="C62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D62">
         <v>2</v>
@@ -1237,7 +1233,7 @@
         <v>33.5</v>
       </c>
       <c r="C63">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D63">
         <v>2</v>
@@ -1251,7 +1247,7 @@
         <v>33.75</v>
       </c>
       <c r="C64">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D64">
         <v>2</v>
@@ -1265,7 +1261,7 @@
         <v>34</v>
       </c>
       <c r="C65">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D65">
         <v>2</v>
@@ -1279,7 +1275,7 @@
         <v>34.25</v>
       </c>
       <c r="C66">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D66">
         <v>2</v>
@@ -1293,7 +1289,7 @@
         <v>34.5</v>
       </c>
       <c r="C67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D67">
         <v>4</v>
@@ -1307,7 +1303,7 @@
         <v>34.75</v>
       </c>
       <c r="C68">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D68">
         <v>4</v>
@@ -1321,7 +1317,7 @@
         <v>35</v>
       </c>
       <c r="C69">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D69">
         <v>4</v>
@@ -1335,7 +1331,7 @@
         <v>35.25</v>
       </c>
       <c r="C70">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D70">
         <v>4</v>
@@ -1349,7 +1345,7 @@
         <v>35.5</v>
       </c>
       <c r="C71">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D71">
         <v>4</v>
@@ -1363,7 +1359,7 @@
         <v>35.75</v>
       </c>
       <c r="C72">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D72">
         <v>4</v>
@@ -1377,7 +1373,7 @@
         <v>36</v>
       </c>
       <c r="C73">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D73">
         <v>4</v>
@@ -1391,7 +1387,7 @@
         <v>36.25</v>
       </c>
       <c r="C74">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D74">
         <v>4</v>
@@ -1405,7 +1401,7 @@
         <v>36.5</v>
       </c>
       <c r="C75">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D75">
         <v>4</v>
@@ -1419,7 +1415,7 @@
         <v>36.75</v>
       </c>
       <c r="C76">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D76">
         <v>4</v>
@@ -1433,7 +1429,7 @@
         <v>37</v>
       </c>
       <c r="C77">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D77">
         <v>4</v>
@@ -1447,7 +1443,7 @@
         <v>37.25</v>
       </c>
       <c r="C78">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D78">
         <v>4</v>
@@ -1461,7 +1457,7 @@
         <v>37.5</v>
       </c>
       <c r="C79">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D79">
         <v>4</v>
@@ -1475,7 +1471,7 @@
         <v>37.75</v>
       </c>
       <c r="C80">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D80">
         <v>4</v>
@@ -1489,7 +1485,7 @@
         <v>38</v>
       </c>
       <c r="C81">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D81">
         <v>4</v>
@@ -1503,7 +1499,7 @@
         <v>38.25</v>
       </c>
       <c r="C82">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D82">
         <v>4</v>
@@ -1517,7 +1513,7 @@
         <v>38.5</v>
       </c>
       <c r="C83">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D83">
         <v>4</v>
@@ -1531,7 +1527,7 @@
         <v>38.75</v>
       </c>
       <c r="C84">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D84">
         <v>4</v>
@@ -1545,7 +1541,7 @@
         <v>39</v>
       </c>
       <c r="C85">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D85">
         <v>4</v>
@@ -1559,7 +1555,7 @@
         <v>39.25</v>
       </c>
       <c r="C86">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D86">
         <v>4</v>
@@ -1573,7 +1569,7 @@
         <v>39.5</v>
       </c>
       <c r="C87">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D87">
         <v>4</v>
@@ -1587,7 +1583,7 @@
         <v>39.75</v>
       </c>
       <c r="C88">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D88">
         <v>4</v>
@@ -1601,7 +1597,7 @@
         <v>40</v>
       </c>
       <c r="C89">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D89">
         <v>4</v>

</xml_diff>